<commit_message>
debug ONE DRIVE DATA LIMIT STORAGE and implement filters on restaraunts
</commit_message>
<xml_diff>
--- a/my-app/public/FoodAR.xlsx
+++ b/my-app/public/FoodAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itayg\OneDrive\Desktop\AR-FoodFinder\my-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51A6056-4A20-46BF-9F01-96F1529E40CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C863B29-65AE-4552-BB57-3DF7887B3D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{DA96FEAB-205F-4F25-B9ED-B68EE0B69310}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -522,6 +522,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fantastic China </t>
+  </si>
+  <si>
+    <t>new2</t>
   </si>
 </sst>
 </file>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B187622D-BC7B-4C02-9F26-3594D4840DF8}">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1180,6 +1183,9 @@
       <c r="F11" t="s">
         <v>136</v>
       </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
       <c r="H11" t="s">
         <v>116</v>
       </c>
@@ -4354,6 +4360,11 @@
       </c>
       <c r="H133" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A134" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>